<commit_message>
add res boundary attack for SEED 2024
</commit_message>
<xml_diff>
--- a/results/SEED_2024/result.xlsx
+++ b/results/SEED_2024/result.xlsx
@@ -474,7 +474,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AR12"/>
+  <dimension ref="A1:AZ12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -558,6 +558,18 @@
       <c r="AP1" s="1" t="n"/>
       <c r="AQ1" s="1" t="n"/>
       <c r="AR1" s="1" t="n"/>
+      <c r="AS1" s="1" t="inlineStr">
+        <is>
+          <t>BOUNDARY</t>
+        </is>
+      </c>
+      <c r="AT1" s="1" t="n"/>
+      <c r="AU1" s="1" t="n"/>
+      <c r="AV1" s="1" t="n"/>
+      <c r="AW1" s="1" t="n"/>
+      <c r="AX1" s="1" t="n"/>
+      <c r="AY1" s="1" t="n"/>
+      <c r="AZ1" s="1" t="n"/>
     </row>
     <row r="2">
       <c r="B2" s="1" t="inlineStr">
@@ -775,6 +787,46 @@
           <t>0.20</t>
         </is>
       </c>
+      <c r="AS2" s="1" t="inlineStr">
+        <is>
+          <t>0.01</t>
+        </is>
+      </c>
+      <c r="AT2" s="1" t="inlineStr">
+        <is>
+          <t>0.02</t>
+        </is>
+      </c>
+      <c r="AU2" s="1" t="inlineStr">
+        <is>
+          <t>0.03</t>
+        </is>
+      </c>
+      <c r="AV2" s="1" t="inlineStr">
+        <is>
+          <t>0.04</t>
+        </is>
+      </c>
+      <c r="AW2" s="1" t="inlineStr">
+        <is>
+          <t>0.05</t>
+        </is>
+      </c>
+      <c r="AX2" s="1" t="inlineStr">
+        <is>
+          <t>0.07</t>
+        </is>
+      </c>
+      <c r="AY2" s="1" t="inlineStr">
+        <is>
+          <t>0.10</t>
+        </is>
+      </c>
+      <c r="AZ2" s="1" t="inlineStr">
+        <is>
+          <t>0.20</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
@@ -924,6 +976,30 @@
       </c>
       <c r="AR4" t="n">
         <v>30.47003173828125</v>
+      </c>
+      <c r="AS4" t="n">
+        <v>4.186208724975586</v>
+      </c>
+      <c r="AT4" t="n">
+        <v>4.249595165252686</v>
+      </c>
+      <c r="AU4" t="n">
+        <v>4.302657604217529</v>
+      </c>
+      <c r="AV4" t="n">
+        <v>4.353903293609619</v>
+      </c>
+      <c r="AW4" t="n">
+        <v>4.388765335083008</v>
+      </c>
+      <c r="AX4" t="n">
+        <v>4.730515480041504</v>
+      </c>
+      <c r="AY4" t="n">
+        <v>5.006624221801758</v>
+      </c>
+      <c r="AZ4" t="n">
+        <v>7.04196310043335</v>
       </c>
     </row>
     <row r="5">
@@ -1059,6 +1135,30 @@
       <c r="AR5" t="n">
         <v>30.70862307642594</v>
       </c>
+      <c r="AS5" t="n">
+        <v>5.322792225955141</v>
+      </c>
+      <c r="AT5" t="n">
+        <v>5.364417903781465</v>
+      </c>
+      <c r="AU5" t="n">
+        <v>5.440529341188144</v>
+      </c>
+      <c r="AV5" t="n">
+        <v>5.47907246362425</v>
+      </c>
+      <c r="AW5" t="n">
+        <v>5.538794076546599</v>
+      </c>
+      <c r="AX5" t="n">
+        <v>5.940059391328488</v>
+      </c>
+      <c r="AY5" t="n">
+        <v>6.324484750621179</v>
+      </c>
+      <c r="AZ5" t="n">
+        <v>8.787343581911573</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n"/>
@@ -1193,6 +1293,30 @@
       <c r="AR6" t="n">
         <v>0.9856973886489868</v>
       </c>
+      <c r="AS6" t="n">
+        <v>0.9996174573898315</v>
+      </c>
+      <c r="AT6" t="n">
+        <v>0.999610960483551</v>
+      </c>
+      <c r="AU6" t="n">
+        <v>0.9995973110198975</v>
+      </c>
+      <c r="AV6" t="n">
+        <v>0.9996079206466675</v>
+      </c>
+      <c r="AW6" t="n">
+        <v>0.9995827674865723</v>
+      </c>
+      <c r="AX6" t="n">
+        <v>0.9994970560073853</v>
+      </c>
+      <c r="AY6" t="n">
+        <v>0.9994394183158875</v>
+      </c>
+      <c r="AZ6" t="n">
+        <v>0.9989516735076904</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
@@ -1330,6 +1454,30 @@
       </c>
       <c r="AR7" t="n">
         <v>33.84486770629883</v>
+      </c>
+      <c r="AS7" t="n">
+        <v>2.768602848052979</v>
+      </c>
+      <c r="AT7" t="n">
+        <v>2.931120872497559</v>
+      </c>
+      <c r="AU7" t="n">
+        <v>3.079442024230957</v>
+      </c>
+      <c r="AV7" t="n">
+        <v>3.175944566726685</v>
+      </c>
+      <c r="AW7" t="n">
+        <v>3.539762020111084</v>
+      </c>
+      <c r="AX7" t="n">
+        <v>4.408213138580322</v>
+      </c>
+      <c r="AY7" t="n">
+        <v>5.126472949981689</v>
+      </c>
+      <c r="AZ7" t="n">
+        <v>8.938190460205078</v>
       </c>
     </row>
     <row r="8">
@@ -1465,6 +1613,30 @@
       <c r="AR8" t="n">
         <v>34.10642594901473</v>
       </c>
+      <c r="AS8" t="n">
+        <v>3.709892173907027</v>
+      </c>
+      <c r="AT8" t="n">
+        <v>3.876880312603415</v>
+      </c>
+      <c r="AU8" t="n">
+        <v>4.108211918417303</v>
+      </c>
+      <c r="AV8" t="n">
+        <v>4.086089909995064</v>
+      </c>
+      <c r="AW8" t="n">
+        <v>4.608258024753505</v>
+      </c>
+      <c r="AX8" t="n">
+        <v>5.58454845737579</v>
+      </c>
+      <c r="AY8" t="n">
+        <v>6.494436964573326</v>
+      </c>
+      <c r="AZ8" t="n">
+        <v>11.17392798280629</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n"/>
@@ -1599,6 +1771,30 @@
       <c r="AR9" t="n">
         <v>0.9795638918876648</v>
       </c>
+      <c r="AS9" t="n">
+        <v>0.9997526407241821</v>
+      </c>
+      <c r="AT9" t="n">
+        <v>0.9997299909591675</v>
+      </c>
+      <c r="AU9" t="n">
+        <v>0.9996969699859619</v>
+      </c>
+      <c r="AV9" t="n">
+        <v>0.9996999502182007</v>
+      </c>
+      <c r="AW9" t="n">
+        <v>0.9996183514595032</v>
+      </c>
+      <c r="AX9" t="n">
+        <v>0.9994405508041382</v>
+      </c>
+      <c r="AY9" t="n">
+        <v>0.9992414116859436</v>
+      </c>
+      <c r="AZ9" t="n">
+        <v>0.9977531433105469</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
@@ -1736,6 +1932,30 @@
       </c>
       <c r="AR10" t="n">
         <v>34.30585098266602</v>
+      </c>
+      <c r="AS10" t="n">
+        <v>2.971150875091553</v>
+      </c>
+      <c r="AT10" t="n">
+        <v>3.163308620452881</v>
+      </c>
+      <c r="AU10" t="n">
+        <v>3.416063070297241</v>
+      </c>
+      <c r="AV10" t="n">
+        <v>3.897083282470703</v>
+      </c>
+      <c r="AW10" t="n">
+        <v>4.299318313598633</v>
+      </c>
+      <c r="AX10" t="n">
+        <v>5.331329822540283</v>
+      </c>
+      <c r="AY10" t="n">
+        <v>6.975700855255127</v>
+      </c>
+      <c r="AZ10" t="n">
+        <v>11.95866680145264</v>
       </c>
     </row>
     <row r="11">
@@ -1871,6 +2091,30 @@
       <c r="AR11" t="n">
         <v>34.50646558244103</v>
       </c>
+      <c r="AS11" t="n">
+        <v>3.831296891241326</v>
+      </c>
+      <c r="AT11" t="n">
+        <v>4.097779365777375</v>
+      </c>
+      <c r="AU11" t="n">
+        <v>4.376790361557034</v>
+      </c>
+      <c r="AV11" t="n">
+        <v>4.945704922164688</v>
+      </c>
+      <c r="AW11" t="n">
+        <v>5.395146428084112</v>
+      </c>
+      <c r="AX11" t="n">
+        <v>6.785276843433952</v>
+      </c>
+      <c r="AY11" t="n">
+        <v>8.638624404614655</v>
+      </c>
+      <c r="AZ11" t="n">
+        <v>15.06382600004944</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="n"/>
@@ -2005,9 +2249,33 @@
       <c r="AR12" t="n">
         <v>0.9813221096992493</v>
       </c>
+      <c r="AS12" t="n">
+        <v>0.9998003244400024</v>
+      </c>
+      <c r="AT12" t="n">
+        <v>0.9997552037239075</v>
+      </c>
+      <c r="AU12" t="n">
+        <v>0.9997143149375916</v>
+      </c>
+      <c r="AV12" t="n">
+        <v>0.9996235966682434</v>
+      </c>
+      <c r="AW12" t="n">
+        <v>0.999544084072113</v>
+      </c>
+      <c r="AX12" t="n">
+        <v>0.9992557764053345</v>
+      </c>
+      <c r="AY12" t="n">
+        <v>0.9987260103225708</v>
+      </c>
+      <c r="AZ12" t="n">
+        <v>0.9959961771965027</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="9">
     <mergeCell ref="M1:T1"/>
     <mergeCell ref="A4:A6"/>
     <mergeCell ref="A7:A9"/>
@@ -2016,6 +2284,7 @@
     <mergeCell ref="AC1:AJ1"/>
     <mergeCell ref="AK1:AR1"/>
     <mergeCell ref="U1:AB1"/>
+    <mergeCell ref="AS1:AZ1"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>